<commit_message>
edicion carpeta analisis y requisitos
Se agrego TCUR
</commit_message>
<xml_diff>
--- a/PROYECTOS/Proy_SSEL/Documentacion/4. Analisis y Diseño/SSEL-TCUR.xlsx
+++ b/PROYECTOS/Proy_SSEL/Documentacion/4. Analisis y Diseño/SSEL-TCUR.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pulpin\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9000" windowHeight="2805"/>
   </bookViews>
@@ -19,16 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Nombre del Caso de Uso</t>
-  </si>
-  <si>
-    <t>Requisitos Funcionales</t>
-  </si>
-  <si>
-    <t>Requisitos no Funcionales</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>CU – 01 Apostar</t>
   </si>
@@ -51,38 +47,35 @@
     <t>RF-03</t>
   </si>
   <si>
-    <t xml:space="preserve">RF-05 </t>
-  </si>
-  <si>
     <t>RF-06</t>
   </si>
   <si>
-    <t xml:space="preserve">RF-04   </t>
-  </si>
-  <si>
-    <t>RF-01, RF-02</t>
-  </si>
-  <si>
-    <t>RNF-09</t>
-  </si>
-  <si>
-    <t>RNF-11</t>
-  </si>
-  <si>
-    <t>RNF-13, RNF-10</t>
-  </si>
-  <si>
-    <t>RNF-12, RNF-14</t>
-  </si>
-  <si>
-    <t>RNF-13,, RNF-14</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>RF-01</t>
+  </si>
+  <si>
+    <t>RF-02</t>
+  </si>
+  <si>
+    <t>RF-04</t>
+  </si>
+  <si>
+    <t>RF-05</t>
+  </si>
+  <si>
+    <t>RF-07</t>
+  </si>
+  <si>
+    <t>RF-08</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,7 +97,14 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="24"/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -168,19 +168,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -204,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -213,15 +200,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -245,16 +233,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>581026</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1647826</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>627857</xdr:rowOff>
+      <xdr:rowOff>580232</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -277,7 +265,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4229101" y="238126"/>
+          <a:off x="7210426" y="190501"/>
           <a:ext cx="1619250" cy="580231"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -545,7 +533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,96 +541,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="2" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>